<commit_message>
Add view of accounts to Customer DB
</commit_message>
<xml_diff>
--- a/RequirementsStatus.xlsx
+++ b/RequirementsStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelgerman/Documents/Revature Oracle Certificate/project-0-LaurelGerman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B39D3A8-C591-624E-9EA4-95CA6006CC9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C79E94-6B63-8F48-BDE8-D1E463BC07D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{7B6832F9-C0E2-1745-9CFF-9315C0497BCD}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Functionality should reflect the below user stories.</t>
   </si>
@@ -106,13 +106,25 @@
     <t>~</t>
   </si>
   <si>
-    <t>Can register when signing up; still need to be able to add once a member</t>
-  </si>
-  <si>
     <t>Need to validate starting balance</t>
   </si>
   <si>
     <t>Currently debugs everything; will want to turn some of this off later</t>
+  </si>
+  <si>
+    <t>Can register both when signing up, and after you're already a member</t>
+  </si>
+  <si>
+    <t>View balance of all accounts at once on Customer DB</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Provide username &amp; password at login</t>
+  </si>
+  <si>
+    <t>Be able to log in and out</t>
   </si>
 </sst>
 </file>
@@ -156,13 +168,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -348,6 +360,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CDE96-CF7E-5543-83FB-0DC355FC7A3F}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,45 +723,45 @@
       <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="28"/>
     </row>
     <row r="5" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="28"/>
     </row>
     <row r="6" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>27</v>
+      <c r="D6" s="22" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -764,17 +788,17 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="26">
         <v>3</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -788,40 +812,42 @@
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="26">
         <v>2</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="24">
         <v>3</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>26</v>
+      <c r="D13" s="22" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="26">
         <v>1</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
@@ -893,8 +919,43 @@
       <c r="C21" s="13"/>
       <c r="D21" s="14"/>
     </row>
+    <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="28"/>
+    </row>
+    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>

</xml_diff>

<commit_message>
Add Employee Dashboard and account approval functionality
</commit_message>
<xml_diff>
--- a/RequirementsStatus.xlsx
+++ b/RequirementsStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelgerman/Documents/Revature Oracle Certificate/project-0-LaurelGerman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB63F7B-4BDF-574D-A661-B092DF56500F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849BB129-3F0E-E743-B6B2-DAFA4C30B987}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1560" windowWidth="30820" windowHeight="17440" xr2:uid="{7B6832F9-C0E2-1745-9CFF-9315C0497BCD}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Functionality should reflect the below user stories.</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Works for initial setup; working for withdrawal/deposit tbd</t>
+  </si>
+  <si>
+    <t>Works, but can't print username for some reason???</t>
   </si>
 </sst>
 </file>
@@ -701,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CDE96-CF7E-5543-83FB-0DC355FC7A3F}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,7 +859,9 @@
       <c r="B14" s="20">
         <v>1</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="D14" s="22" t="s">
         <v>27</v>
       </c>
@@ -868,7 +873,9 @@
       <c r="B15" s="24">
         <v>2</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" s="22"/>
     </row>
     <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -886,14 +893,18 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="18">
         <v>2</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="C17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">

</xml_diff>

<commit_message>
Vastly simplify account signup by overriding run() instead of formatting Questions in the constructor
</commit_message>
<xml_diff>
--- a/RequirementsStatus.xlsx
+++ b/RequirementsStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelgerman/Documents/Revature Oracle Certificate/project-0-LaurelGerman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D085280-B06D-7A44-AFA6-741B9827D076}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB856D2-3465-9B40-9348-7A75F34E8FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1560" windowWidth="30820" windowHeight="17440" xr2:uid="{7B6832F9-C0E2-1745-9CFF-9315C0497BCD}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Functionality should reflect the below user stories.</t>
   </si>
@@ -106,9 +106,6 @@
     <t>~</t>
   </si>
   <si>
-    <t>Need to validate starting balance</t>
-  </si>
-  <si>
     <t>Currently debugs everything; will want to turn some of this off later</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
   </si>
   <si>
     <t>Be able to log in and out</t>
-  </si>
-  <si>
-    <t>Can register both when signing up; not registering in database when you try to add an account as an existing member</t>
   </si>
   <si>
     <t>Works for initial setup; working for withdrawal/deposit tbd</t>
@@ -385,7 +379,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -704,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CDE96-CF7E-5543-83FB-0DC355FC7A3F}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,7 +770,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -803,18 +797,16 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="24">
         <v>3</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>31</v>
-      </c>
+      <c r="C10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
@@ -839,18 +831,16 @@
       <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="24">
         <v>3</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>25</v>
-      </c>
+      <c r="C13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
@@ -863,7 +853,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -889,7 +879,7 @@
         <v>24</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -903,7 +893,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -949,7 +939,7 @@
     <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
@@ -961,7 +951,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="21" t="s">
@@ -971,7 +961,7 @@
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="25" t="s">

</xml_diff>

<commit_message>
Add functionality to view accounts
</commit_message>
<xml_diff>
--- a/RequirementsStatus.xlsx
+++ b/RequirementsStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelgerman/Documents/Revature Oracle Certificate/project-0-LaurelGerman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB856D2-3465-9B40-9348-7A75F34E8FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B54B0D3-55C5-D84C-AA65-D3495205912C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1560" windowWidth="30820" windowHeight="17440" xr2:uid="{7B6832F9-C0E2-1745-9CFF-9315C0497BCD}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Functionality should reflect the below user stories.</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>Be able to log in and out</t>
-  </si>
-  <si>
-    <t>Works for initial setup; working for withdrawal/deposit tbd</t>
   </si>
   <si>
     <t>Works, but can't print username for some reason???</t>
@@ -698,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CDE96-CF7E-5543-83FB-0DC355FC7A3F}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,18 +866,16 @@
       <c r="D15" s="22"/>
     </row>
     <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="24">
         <v>2</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>30</v>
-      </c>
+      <c r="C16" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="22"/>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
@@ -893,18 +888,20 @@
         <v>24</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="24">
         <v>1</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
+      <c r="C18" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">

</xml_diff>

<commit_message>
Add transaction logging for employee view
</commit_message>
<xml_diff>
--- a/RequirementsStatus.xlsx
+++ b/RequirementsStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelgerman/Documents/Revature Oracle Certificate/project-0-LaurelGerman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8329A7AB-5218-7A4A-A4E6-E5542EA7847B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265B444-FF91-AD40-9A63-1487F41B6E9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1560" windowWidth="30820" windowHeight="17440" xr2:uid="{7B6832F9-C0E2-1745-9CFF-9315C0497BCD}"/>
   </bookViews>
@@ -298,13 +298,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -338,6 +332,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CDE96-CF7E-5543-83FB-0DC355FC7A3F}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,40 +727,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="28"/>
-      <c r="C3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="22"/>
+      <c r="C3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="28"/>
-      <c r="C4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="22"/>
+      <c r="C4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="28"/>
-      <c r="C5" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="22"/>
+      <c r="C5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="28"/>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>25</v>
       </c>
     </row>
@@ -769,8 +769,8 @@
         <v>5</v>
       </c>
       <c r="B7" s="34"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -788,13 +788,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="22">
         <v>3</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="35"/>
@@ -810,124 +810,124 @@
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="18">
         <v>2</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="22"/>
+      <c r="C12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="22">
         <v>3</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="22"/>
+      <c r="C13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="18">
         <v>1</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="22"/>
+      <c r="C14" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="20"/>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="22">
         <v>2</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="22"/>
+      <c r="C15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="22">
         <v>2</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="22"/>
+      <c r="C16" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <v>2</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="22">
         <v>1</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="22"/>
+      <c r="C18" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="20"/>
     </row>
     <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="22">
         <v>3</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="22">
         <v>2</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="24">
         <v>2</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -947,10 +947,10 @@
         <v>27</v>
       </c>
       <c r="B24" s="28"/>
-      <c r="C24" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="22"/>
+      <c r="C24" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="20"/>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">

</xml_diff>

<commit_message>
Add 10 junit tests
</commit_message>
<xml_diff>
--- a/RequirementsStatus.xlsx
+++ b/RequirementsStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelgerman/Documents/Revature Oracle Certificate/project-0-LaurelGerman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265B444-FF91-AD40-9A63-1487F41B6E9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3993229B-3CD0-1142-A192-1AA26BBF4535}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1560" windowWidth="30820" windowHeight="17440" xr2:uid="{7B6832F9-C0E2-1745-9CFF-9315C0497BCD}"/>
   </bookViews>
@@ -268,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -298,12 +298,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -356,18 +350,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -690,7 +672,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:D21"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -715,62 +697,62 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="20"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="20"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="20"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -788,16 +770,16 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>3</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="35"/>
+      <c r="C10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
@@ -810,124 +792,124 @@
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="16">
         <v>2</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="20"/>
+      <c r="C12" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="20">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="20"/>
+      <c r="C13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="16">
         <v>1</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="20"/>
+      <c r="C14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="20">
         <v>2</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="20"/>
+      <c r="C15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="20">
         <v>2</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="20"/>
+      <c r="C16" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="14">
         <v>2</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="20">
         <v>1</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="20"/>
+      <c r="C18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="20">
         <v>3</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20" t="s">
+      <c r="C19" s="17"/>
+      <c r="D19" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="20">
         <v>2</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20" t="s">
+      <c r="C20" s="17"/>
+      <c r="D20" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="22">
         <v>2</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
     </row>
     <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -943,24 +925,24 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="20"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="26"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Add joint account functionality
</commit_message>
<xml_diff>
--- a/RequirementsStatus.xlsx
+++ b/RequirementsStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelgerman/Documents/Revature Oracle Certificate/project-0-LaurelGerman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3993229B-3CD0-1142-A192-1AA26BBF4535}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEA24FC-30AC-B44C-8611-62691DDE52EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1560" windowWidth="30820" windowHeight="17440" xr2:uid="{7B6832F9-C0E2-1745-9CFF-9315C0497BCD}"/>
   </bookViews>
@@ -671,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CDE96-CF7E-5543-83FB-0DC355FC7A3F}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add powerpoint slides and finishing touches
</commit_message>
<xml_diff>
--- a/RequirementsStatus.xlsx
+++ b/RequirementsStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelgerman/Documents/Revature Oracle Certificate/project-0-LaurelGerman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEA24FC-30AC-B44C-8611-62691DDE52EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E575FD14-0C0E-754F-90A4-31FF5C837E4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1560" windowWidth="30820" windowHeight="17440" xr2:uid="{7B6832F9-C0E2-1745-9CFF-9315C0497BCD}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Functionality should reflect the below user stories.</t>
   </si>
@@ -268,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -284,18 +284,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -671,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CDE96-CF7E-5543-83FB-0DC355FC7A3F}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,62 +685,62 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="18"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="18"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="18"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -770,146 +758,148 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="16">
         <v>3</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="29"/>
+      <c r="C10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="16">
         <v>3</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="12">
         <v>2</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="18"/>
+      <c r="C12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="16">
         <v>3</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="18"/>
+      <c r="C13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="12">
         <v>1</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="18"/>
+      <c r="C14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="16">
         <v>2</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="18"/>
+      <c r="C15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="16">
         <v>2</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="18"/>
+      <c r="C16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="10">
         <v>2</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="16">
         <v>1</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="18"/>
+      <c r="C18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="16">
         <v>3</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="16">
         <v>2</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18" t="s">
+      <c r="C20" s="13"/>
+      <c r="D20" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="18">
         <v>2</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -925,24 +915,24 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="18"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>